<commit_message>
Update BOM and CPL for order
</commit_message>
<xml_diff>
--- a/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
+++ b/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\datMach\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB459914-8C4B-4C7B-A0DB-8D95F62D2C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9375"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -736,7 +742,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -842,6 +848,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1104,11 +1113,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E150"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="F143" sqref="F143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1664,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>38</v>
       </c>
@@ -1681,7 +1690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -1698,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>40</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>41</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>42</v>
       </c>
@@ -1746,10 +1755,10 @@
         <v>6</v>
       </c>
       <c r="E37" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>43</v>
       </c>
@@ -1763,10 +1772,10 @@
         <v>6</v>
       </c>
       <c r="E38" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>44</v>
       </c>
@@ -1780,10 +1789,10 @@
         <v>6</v>
       </c>
       <c r="E39" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>45</v>
       </c>
@@ -1797,10 +1806,10 @@
         <v>6</v>
       </c>
       <c r="E40" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
         <v>46</v>
       </c>
@@ -1814,10 +1823,10 @@
         <v>6</v>
       </c>
       <c r="E41" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>47</v>
       </c>
@@ -1831,10 +1840,10 @@
         <v>6</v>
       </c>
       <c r="E42" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>48</v>
       </c>
@@ -1848,10 +1857,10 @@
         <v>6</v>
       </c>
       <c r="E43" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>49</v>
       </c>
@@ -1865,10 +1874,10 @@
         <v>6</v>
       </c>
       <c r="E44" s="8">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>50</v>
       </c>
@@ -1882,10 +1891,11 @@
         <v>6</v>
       </c>
       <c r="E45" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
@@ -1899,10 +1909,11 @@
         <v>6</v>
       </c>
       <c r="E46" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="14.25" customHeight="1">
+        <v>270</v>
+      </c>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6" ht="14.25" customHeight="1">
       <c r="A47" s="4" t="s">
         <v>52</v>
       </c>
@@ -1916,10 +1927,11 @@
         <v>6</v>
       </c>
       <c r="E47" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
@@ -1933,10 +1945,11 @@
         <v>6</v>
       </c>
       <c r="E48" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
@@ -1950,10 +1963,11 @@
         <v>6</v>
       </c>
       <c r="E49" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
         <v>55</v>
       </c>
@@ -1967,10 +1981,11 @@
         <v>6</v>
       </c>
       <c r="E50" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
@@ -1984,10 +1999,11 @@
         <v>6</v>
       </c>
       <c r="E51" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
@@ -2001,10 +2017,11 @@
         <v>6</v>
       </c>
       <c r="E52" s="8">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>270</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -2021,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>59</v>
       </c>
@@ -2038,7 +2055,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
         <v>9</v>
       </c>
@@ -2055,7 +2072,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
         <v>60</v>
       </c>
@@ -2072,7 +2089,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
         <v>61</v>
       </c>
@@ -2089,7 +2106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
         <v>62</v>
       </c>
@@ -2106,7 +2123,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
         <v>63</v>
       </c>
@@ -2123,7 +2140,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:5">
+    <row r="60" spans="1:6">
       <c r="A60" s="4" t="s">
         <v>64</v>
       </c>
@@ -2140,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5">
+    <row r="61" spans="1:6">
       <c r="A61" s="4" t="s">
         <v>65</v>
       </c>
@@ -2157,7 +2174,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:5">
+    <row r="62" spans="1:6">
       <c r="A62" s="9" t="s">
         <v>66</v>
       </c>
@@ -2174,7 +2191,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
         <v>67</v>
       </c>
@@ -2191,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
         <v>68</v>
       </c>
@@ -3548,7 +3565,7 @@
         <v>6</v>
       </c>
       <c r="E143" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3565,7 +3582,7 @@
         <v>6</v>
       </c>
       <c r="E144" s="8">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3582,7 +3599,7 @@
         <v>6</v>
       </c>
       <c r="E145" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3599,7 +3616,7 @@
         <v>6</v>
       </c>
       <c r="E146" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3616,7 +3633,7 @@
         <v>6</v>
       </c>
       <c r="E147" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3633,7 +3650,7 @@
         <v>6</v>
       </c>
       <c r="E148" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3650,7 +3667,7 @@
         <v>6</v>
       </c>
       <c r="E149" s="8">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="150" spans="1:5">

</xml_diff>

<commit_message>
Add new footprint for led and button reset again
</commit_message>
<xml_diff>
--- a/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
+++ b/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\datMach\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB459914-8C4B-4C7B-A0DB-8D95F62D2C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2859AAB8-D01C-4316-BE2D-CD2259FC2F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="243">
   <si>
     <t>Designator</t>
   </si>
@@ -568,27 +568,12 @@
     <t>50.0000mm</t>
   </si>
   <si>
-    <t>162.0000mm</t>
-  </si>
-  <si>
     <t>152.0000mm</t>
   </si>
   <si>
-    <t>142.0000mm</t>
-  </si>
-  <si>
     <t>132.0000mm</t>
   </si>
   <si>
-    <t>122.0000mm</t>
-  </si>
-  <si>
-    <t>112.0000mm</t>
-  </si>
-  <si>
-    <t>102.0000mm</t>
-  </si>
-  <si>
     <t>92.0000mm</t>
   </si>
   <si>
@@ -737,6 +722,33 @@
   </si>
   <si>
     <t>TD0</t>
+  </si>
+  <si>
+    <t>92.3290mm</t>
+  </si>
+  <si>
+    <t>25.0190mm</t>
+  </si>
+  <si>
+    <t>102.3620mm</t>
+  </si>
+  <si>
+    <t>142.3670mm</t>
+  </si>
+  <si>
+    <t>112.3950mm</t>
+  </si>
+  <si>
+    <t>132.4610mm</t>
+  </si>
+  <si>
+    <t>122.4280mm</t>
+  </si>
+  <si>
+    <t>152.4000mm</t>
+  </si>
+  <si>
+    <t>162.4330mm</t>
   </si>
 </sst>
 </file>
@@ -1116,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="F143" sqref="F143"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1610,10 +1622,10 @@
         <v>34</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>6</v>
@@ -1627,10 +1639,10 @@
         <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>183</v>
+        <v>241</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>6</v>
@@ -1644,10 +1656,10 @@
         <v>36</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>6</v>
@@ -1661,10 +1673,10 @@
         <v>37</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>185</v>
+        <v>239</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>6</v>
@@ -1678,10 +1690,10 @@
         <v>38</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>6</v>
@@ -1695,10 +1707,10 @@
         <v>39</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>6</v>
@@ -1712,10 +1724,10 @@
         <v>40</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>188</v>
+        <v>236</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>6</v>
@@ -1729,10 +1741,10 @@
         <v>41</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>189</v>
+        <v>234</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>158</v>
+        <v>235</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>6</v>
@@ -1746,10 +1758,10 @@
         <v>42</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>6</v>
@@ -1763,10 +1775,10 @@
         <v>43</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -1780,10 +1792,10 @@
         <v>44</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>6</v>
@@ -1797,10 +1809,10 @@
         <v>45</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>6</v>
@@ -1814,10 +1826,10 @@
         <v>46</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>6</v>
@@ -1831,10 +1843,10 @@
         <v>47</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>6</v>
@@ -1851,7 +1863,7 @@
         <v>153</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>6</v>
@@ -1865,10 +1877,10 @@
         <v>49</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>6</v>
@@ -1885,7 +1897,7 @@
         <v>165</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>6</v>
@@ -1903,7 +1915,7 @@
         <v>160</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>6</v>
@@ -1921,7 +1933,7 @@
         <v>172</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>6</v>
@@ -1939,7 +1951,7 @@
         <v>174</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>6</v>
@@ -1957,7 +1969,7 @@
         <v>175</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>6</v>
@@ -1975,7 +1987,7 @@
         <v>176</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>6</v>
@@ -1993,7 +2005,7 @@
         <v>177</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>6</v>
@@ -2011,7 +2023,7 @@
         <v>178</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>6</v>
@@ -2026,10 +2038,10 @@
         <v>58</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>6</v>
@@ -2094,7 +2106,7 @@
         <v>61</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>178</v>
@@ -2111,10 +2123,10 @@
         <v>62</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>6</v>
@@ -2128,10 +2140,10 @@
         <v>63</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>6</v>
@@ -2145,7 +2157,7 @@
         <v>64</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>178</v>
@@ -2162,10 +2174,10 @@
         <v>65</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>6</v>
@@ -2179,10 +2191,10 @@
         <v>66</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>6</v>
@@ -2196,7 +2208,7 @@
         <v>67</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>178</v>
@@ -2213,10 +2225,10 @@
         <v>68</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>6</v>
@@ -2230,10 +2242,10 @@
         <v>69</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>6</v>
@@ -2247,7 +2259,7 @@
         <v>70</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>178</v>
@@ -2264,10 +2276,10 @@
         <v>71</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>6</v>
@@ -2281,10 +2293,10 @@
         <v>72</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>6</v>
@@ -2298,7 +2310,7 @@
         <v>73</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>178</v>
@@ -2315,10 +2327,10 @@
         <v>74</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>6</v>
@@ -2332,10 +2344,10 @@
         <v>75</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>6</v>
@@ -2349,7 +2361,7 @@
         <v>76</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>178</v>
@@ -2366,10 +2378,10 @@
         <v>77</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>6</v>
@@ -2380,13 +2392,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>6</v>
@@ -2400,7 +2412,7 @@
         <v>79</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>178</v>
@@ -2417,10 +2429,10 @@
         <v>80</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>6</v>
@@ -2434,10 +2446,10 @@
         <v>81</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>6</v>
@@ -2451,7 +2463,7 @@
         <v>82</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>178</v>
@@ -2468,10 +2480,10 @@
         <v>83</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>6</v>
@@ -2485,10 +2497,10 @@
         <v>84</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>6</v>
@@ -2522,7 +2534,7 @@
         <v>165</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>6</v>
@@ -2539,7 +2551,7 @@
         <v>165</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>6</v>
@@ -2573,7 +2585,7 @@
         <v>160</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>6</v>
@@ -2590,7 +2602,7 @@
         <v>160</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>6</v>
@@ -2624,7 +2636,7 @@
         <v>172</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>6</v>
@@ -2641,7 +2653,7 @@
         <v>172</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>6</v>
@@ -2675,7 +2687,7 @@
         <v>174</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>6</v>
@@ -2692,7 +2704,7 @@
         <v>174</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>6</v>
@@ -2726,7 +2738,7 @@
         <v>175</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>6</v>
@@ -2743,7 +2755,7 @@
         <v>175</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>6</v>
@@ -2777,7 +2789,7 @@
         <v>176</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>6</v>
@@ -2794,7 +2806,7 @@
         <v>176</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>6</v>
@@ -2828,7 +2840,7 @@
         <v>177</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>6</v>
@@ -2845,7 +2857,7 @@
         <v>177</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>6</v>
@@ -2879,7 +2891,7 @@
         <v>178</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>6</v>
@@ -2896,7 +2908,7 @@
         <v>178</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>6</v>
@@ -2910,7 +2922,7 @@
         <v>108</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>154</v>
@@ -2927,7 +2939,7 @@
         <v>109</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>154</v>
@@ -2944,7 +2956,7 @@
         <v>110</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>154</v>
@@ -2961,7 +2973,7 @@
         <v>111</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>154</v>
@@ -2978,7 +2990,7 @@
         <v>112</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>154</v>
@@ -3012,7 +3024,7 @@
         <v>114</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>164</v>
@@ -3046,10 +3058,10 @@
         <v>116</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C113" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>6</v>
@@ -3063,10 +3075,10 @@
         <v>117</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C114" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>6</v>
@@ -3080,10 +3092,10 @@
         <v>118</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>6</v>
@@ -3097,10 +3109,10 @@
         <v>119</v>
       </c>
       <c r="B116" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>224</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>6</v>
@@ -3114,10 +3126,10 @@
         <v>120</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>6</v>
@@ -3131,10 +3143,10 @@
         <v>121</v>
       </c>
       <c r="B118" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C118" s="8" t="s">
         <v>221</v>
-      </c>
-      <c r="C118" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>6</v>
@@ -3148,10 +3160,10 @@
         <v>122</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>6</v>
@@ -3165,10 +3177,10 @@
         <v>123</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>6</v>
@@ -3182,10 +3194,10 @@
         <v>124</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>6</v>
@@ -3199,10 +3211,10 @@
         <v>125</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>6</v>
@@ -3216,10 +3228,10 @@
         <v>126</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>6</v>
@@ -3233,10 +3245,10 @@
         <v>127</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>6</v>
@@ -3250,10 +3262,10 @@
         <v>128</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>6</v>
@@ -3267,10 +3279,10 @@
         <v>129</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>6</v>
@@ -3284,10 +3296,10 @@
         <v>130</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>6</v>
@@ -3301,10 +3313,10 @@
         <v>131</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>6</v>
@@ -3318,10 +3330,10 @@
         <v>132</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>6</v>
@@ -3335,10 +3347,10 @@
         <v>133</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>6</v>
@@ -3352,10 +3364,10 @@
         <v>134</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>6</v>
@@ -3369,10 +3381,10 @@
         <v>135</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>6</v>
@@ -3386,10 +3398,10 @@
         <v>137</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>6</v>
@@ -3403,10 +3415,10 @@
         <v>136</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>6</v>
@@ -3420,10 +3432,10 @@
         <v>138</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>6</v>
@@ -3437,10 +3449,10 @@
         <v>139</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>6</v>
@@ -3454,10 +3466,10 @@
         <v>140</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>6</v>
@@ -3471,10 +3483,10 @@
         <v>141</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>6</v>
@@ -3488,10 +3500,10 @@
         <v>142</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>6</v>
@@ -3505,10 +3517,10 @@
         <v>143</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>6</v>
@@ -3522,10 +3534,10 @@
         <v>144</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>6</v>
@@ -3539,10 +3551,10 @@
         <v>145</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>6</v>
@@ -3553,13 +3565,13 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="9" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B143" s="8" t="s">
         <v>158</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>6</v>
@@ -3573,10 +3585,10 @@
         <v>146</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>6</v>
@@ -3607,10 +3619,10 @@
         <v>148</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>6</v>
@@ -3624,10 +3636,10 @@
         <v>149</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>6</v>
@@ -3641,10 +3653,10 @@
         <v>150</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>6</v>
@@ -3658,10 +3670,10 @@
         <v>151</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>6</v>
@@ -3672,7 +3684,7 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="9" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B150" s="8" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
Fix error un similar between schematic and jlc
</commit_message>
<xml_diff>
--- a/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
+++ b/digitalSystemBoard/JLCSMT_DigitalSystemBoard_CPL1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\digitalSystemBoard\digitalSystemBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2859AAB8-D01C-4316-BE2D-CD2259FC2F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FDCD5E-5980-420D-8CBF-32FF9C613F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>D7</t>
   </si>
   <si>
-    <t>FB0</t>
-  </si>
-  <si>
     <t>FB1</t>
   </si>
   <si>
@@ -749,6 +746,9 @@
   </si>
   <si>
     <t>162.4330mm</t>
+  </si>
+  <si>
+    <t>FB6</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1163,10 +1163,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>6</v>
@@ -1180,10 +1180,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
@@ -1197,10 +1197,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
@@ -1214,10 +1214,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>6</v>
@@ -1231,10 +1231,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>6</v>
@@ -1248,10 +1248,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>6</v>
@@ -1265,10 +1265,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>161</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>6</v>
@@ -1282,10 +1282,10 @@
         <v>14</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>6</v>
@@ -1299,10 +1299,10 @@
         <v>15</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>6</v>
@@ -1316,10 +1316,10 @@
         <v>16</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>6</v>
@@ -1333,10 +1333,10 @@
         <v>17</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>6</v>
@@ -1350,10 +1350,10 @@
         <v>18</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>169</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>6</v>
@@ -1367,10 +1367,10 @@
         <v>19</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>6</v>
@@ -1384,10 +1384,10 @@
         <v>20</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>6</v>
@@ -1401,10 +1401,10 @@
         <v>21</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>6</v>
@@ -1418,10 +1418,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>6</v>
@@ -1435,10 +1435,10 @@
         <v>23</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>6</v>
@@ -1452,10 +1452,10 @@
         <v>24</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>6</v>
@@ -1469,10 +1469,10 @@
         <v>25</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>6</v>
@@ -1486,10 +1486,10 @@
         <v>26</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>6</v>
@@ -1503,10 +1503,10 @@
         <v>27</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>6</v>
@@ -1520,16 +1520,16 @@
         <v>28</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="8">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1537,10 +1537,10 @@
         <v>29</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>6</v>
@@ -1554,16 +1554,16 @@
         <v>30</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E25" s="8">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1571,10 +1571,10 @@
         <v>31</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>6</v>
@@ -1588,27 +1588,27 @@
         <v>32</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="8">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="4" t="s">
-        <v>33</v>
+        <v>242</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>6</v>
@@ -1619,13 +1619,13 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>6</v>
@@ -1636,13 +1636,13 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>6</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>6</v>
@@ -1670,13 +1670,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>6</v>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>6</v>
@@ -1704,13 +1704,13 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>6</v>
@@ -1721,13 +1721,13 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>6</v>
@@ -1738,13 +1738,13 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>234</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>235</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>6</v>
@@ -1755,13 +1755,13 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>6</v>
@@ -1772,13 +1772,13 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>6</v>
@@ -1789,13 +1789,13 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>6</v>
@@ -1806,13 +1806,13 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>6</v>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>6</v>
@@ -1840,13 +1840,13 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>6</v>
@@ -1857,13 +1857,13 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>6</v>
@@ -1874,13 +1874,13 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>6</v>
@@ -1891,13 +1891,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>6</v>
@@ -1909,13 +1909,13 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>6</v>
@@ -1927,13 +1927,13 @@
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1">
       <c r="A47" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>6</v>
@@ -1945,13 +1945,13 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>6</v>
@@ -1963,13 +1963,13 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>6</v>
@@ -1981,13 +1981,13 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>6</v>
@@ -1999,13 +1999,13 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>6</v>
@@ -2017,13 +2017,13 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>6</v>
@@ -2035,13 +2035,13 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>194</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>195</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>6</v>
@@ -2052,13 +2052,13 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>6</v>
@@ -2072,10 +2072,10 @@
         <v>9</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>6</v>
@@ -2086,13 +2086,13 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>6</v>
@@ -2103,13 +2103,13 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>6</v>
@@ -2120,13 +2120,13 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>6</v>
@@ -2137,13 +2137,13 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>6</v>
@@ -2154,13 +2154,13 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>6</v>
@@ -2171,13 +2171,13 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>6</v>
@@ -2188,13 +2188,13 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>6</v>
@@ -2205,13 +2205,13 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>6</v>
@@ -2222,13 +2222,13 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>6</v>
@@ -2239,13 +2239,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>6</v>
@@ -2256,13 +2256,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C66" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>6</v>
@@ -2273,13 +2273,13 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>6</v>
@@ -2290,13 +2290,13 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>6</v>
@@ -2307,13 +2307,13 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C69" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>6</v>
@@ -2324,13 +2324,13 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>6</v>
@@ -2341,13 +2341,13 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>6</v>
@@ -2358,13 +2358,13 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C72" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>6</v>
@@ -2375,13 +2375,13 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>6</v>
@@ -2392,13 +2392,13 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C74" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>6</v>
@@ -2409,13 +2409,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>6</v>
@@ -2426,13 +2426,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>6</v>
@@ -2443,13 +2443,13 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C77" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>6</v>
@@ -2460,13 +2460,13 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>6</v>
@@ -2477,13 +2477,13 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>6</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C80" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>6</v>
@@ -2511,13 +2511,13 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C81" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>6</v>
@@ -2528,13 +2528,13 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>6</v>
@@ -2545,13 +2545,13 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>6</v>
@@ -2562,13 +2562,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C84" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>6</v>
@@ -2579,13 +2579,13 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C85" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>6</v>
@@ -2596,13 +2596,13 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C86" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>6</v>
@@ -2613,13 +2613,13 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>6</v>
@@ -2630,13 +2630,13 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C88" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>6</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>6</v>
@@ -2664,13 +2664,13 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C90" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>6</v>
@@ -2681,13 +2681,13 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C91" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>6</v>
@@ -2698,13 +2698,13 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C92" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>6</v>
@@ -2715,13 +2715,13 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C93" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>6</v>
@@ -2732,13 +2732,13 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>6</v>
@@ -2749,13 +2749,13 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C95" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>6</v>
@@ -2766,13 +2766,13 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>6</v>
@@ -2783,13 +2783,13 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C97" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>6</v>
@@ -2800,13 +2800,13 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C98" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>6</v>
@@ -2817,13 +2817,13 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B99" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C99" s="8" t="s">
         <v>177</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>178</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>6</v>
@@ -2834,13 +2834,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>6</v>
@@ -2851,13 +2851,13 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C101" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>6</v>
@@ -2868,13 +2868,13 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C102" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>6</v>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>6</v>
@@ -2902,13 +2902,13 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C104" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>6</v>
@@ -2919,13 +2919,13 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C105" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>6</v>
@@ -2936,13 +2936,13 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C106" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>6</v>
@@ -2953,13 +2953,13 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>6</v>
@@ -2970,13 +2970,13 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C108" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>6</v>
@@ -2987,13 +2987,13 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C109" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>6</v>
@@ -3004,13 +3004,13 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>6</v>
@@ -3021,13 +3021,13 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C111" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>6</v>
@@ -3038,13 +3038,13 @@
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C112" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>6</v>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B113" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>215</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>6</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>216</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>217</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>6</v>
@@ -3089,13 +3089,13 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>6</v>
@@ -3106,13 +3106,13 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>6</v>
@@ -3123,13 +3123,13 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>6</v>
@@ -3140,13 +3140,13 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>6</v>
@@ -3157,13 +3157,13 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C119" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>6</v>
@@ -3174,13 +3174,13 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C120" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>6</v>
@@ -3191,13 +3191,13 @@
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C121" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>6</v>
@@ -3208,13 +3208,13 @@
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C122" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>6</v>
@@ -3225,13 +3225,13 @@
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C123" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>6</v>
@@ -3242,13 +3242,13 @@
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>6</v>
@@ -3259,13 +3259,13 @@
     </row>
     <row r="125" spans="1:5">
       <c r="A125" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>6</v>
@@ -3276,13 +3276,13 @@
     </row>
     <row r="126" spans="1:5">
       <c r="A126" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>6</v>
@@ -3293,13 +3293,13 @@
     </row>
     <row r="127" spans="1:5">
       <c r="A127" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C127" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>6</v>
@@ -3310,13 +3310,13 @@
     </row>
     <row r="128" spans="1:5">
       <c r="A128" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C128" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>6</v>
@@ -3327,13 +3327,13 @@
     </row>
     <row r="129" spans="1:5">
       <c r="A129" s="9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C129" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>6</v>
@@ -3344,13 +3344,13 @@
     </row>
     <row r="130" spans="1:5">
       <c r="A130" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C130" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>6</v>
@@ -3361,13 +3361,13 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C131" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>6</v>
@@ -3378,13 +3378,13 @@
     </row>
     <row r="132" spans="1:5">
       <c r="A132" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>6</v>
@@ -3395,13 +3395,13 @@
     </row>
     <row r="133" spans="1:5">
       <c r="A133" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>6</v>
@@ -3412,13 +3412,13 @@
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>6</v>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B135" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>6</v>
@@ -3446,13 +3446,13 @@
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D136" s="5" t="s">
         <v>6</v>
@@ -3463,13 +3463,13 @@
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>6</v>
@@ -3480,13 +3480,13 @@
     </row>
     <row r="138" spans="1:5">
       <c r="A138" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D138" s="5" t="s">
         <v>6</v>
@@ -3497,13 +3497,13 @@
     </row>
     <row r="139" spans="1:5">
       <c r="A139" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C139" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D139" s="5" t="s">
         <v>6</v>
@@ -3514,13 +3514,13 @@
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D140" s="5" t="s">
         <v>6</v>
@@ -3531,13 +3531,13 @@
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C141" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D141" s="5" t="s">
         <v>6</v>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D142" s="5" t="s">
         <v>6</v>
@@ -3565,13 +3565,13 @@
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D143" s="5" t="s">
         <v>6</v>
@@ -3582,13 +3582,13 @@
     </row>
     <row r="144" spans="1:5">
       <c r="A144" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C144" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D144" s="5" t="s">
         <v>6</v>
@@ -3599,13 +3599,13 @@
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C145" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D145" s="5" t="s">
         <v>6</v>
@@ -3616,13 +3616,13 @@
     </row>
     <row r="146" spans="1:5">
       <c r="A146" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C146" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D146" s="5" t="s">
         <v>6</v>
@@ -3633,13 +3633,13 @@
     </row>
     <row r="147" spans="1:5">
       <c r="A147" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C147" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D147" s="5" t="s">
         <v>6</v>
@@ -3650,13 +3650,13 @@
     </row>
     <row r="148" spans="1:5">
       <c r="A148" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C148" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D148" s="5" t="s">
         <v>6</v>
@@ -3667,13 +3667,13 @@
     </row>
     <row r="149" spans="1:5">
       <c r="A149" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C149" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D149" s="5" t="s">
         <v>6</v>
@@ -3684,13 +3684,13 @@
     </row>
     <row r="150" spans="1:5">
       <c r="A150" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C150" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D150" s="5" t="s">
         <v>6</v>

</xml_diff>